<commit_message>
minor update to bom
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t xml:space="preserve">Item #</t>
   </si>
@@ -79,13 +79,16 @@
     <t xml:space="preserve">16-SOIC</t>
   </si>
   <si>
-    <t xml:space="preserve">D7,D5,D2,D4,D10,D1,D9,D6,D8,D11,D3</t>
+    <t xml:space="preserve">D1,D2,D3,D4,D5,D6,D7,D8,D9,D10,D11</t>
   </si>
   <si>
     <t xml:space="preserve">Würth Elektronik</t>
   </si>
   <si>
     <t xml:space="preserve">150060VS75000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED GREEN CLEAR 0603 SMD</t>
   </si>
   <si>
     <t xml:space="preserve">0603</t>
@@ -149,6 +152,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -170,6 +174,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -227,28 +232,32 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -329,45 +338,45 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="33.42"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="33.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="24.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="19.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="33.66"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="30.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="5" customFormat="true" ht="30.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -375,25 +384,25 @@
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -401,25 +410,25 @@
       <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -427,25 +436,25 @@
       <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="5" t="s">
+      <c r="F4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="G4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -453,25 +462,25 @@
       <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>23</v>
+      <c r="B5" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="0" t="s">
+      <c r="D5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="E5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="F5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="G5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -479,25 +488,25 @@
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>28</v>
+      <c r="B6" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="0" t="s">
+      <c r="D6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="0" t="s">
+      <c r="F6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -505,25 +514,25 @@
       <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>31</v>
+      <c r="B7" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="0" t="s">
+      <c r="D7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="E7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="0" t="s">
+      <c r="F7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -531,32 +540,26 @@
       <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>35</v>
+      <c r="B8" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="0" t="s">
+      <c r="D8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="1" t="n">
-        <f aca="false">SUM(C2:C8)</f>
-        <v>20</v>
+      <c r="F8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>